<commit_message>
Atualização das tabelas fatos
Atualização das tabelas fatos 19/10
</commit_message>
<xml_diff>
--- a/Registro de Óbitos BR.xlsx
+++ b/Registro de Óbitos BR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\OneDrive\Documentos\Análise de Dados e afins\Projetos\Covid BR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\OneDrive\Documentos\GitHub\Covid-19_Brasil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A26247-9EC0-4F1B-BCD8-3D7B171CF003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D380B806-DD7F-410B-8C6B-5FCDDE8F6329}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{14E435B9-7256-4543-A568-0AD7A200546E}"/>
   </bookViews>
@@ -8303,8 +8303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C26417B-7ABD-4A0E-AF65-6C704DCE5E36}">
   <dimension ref="B1:U1567"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1533" workbookViewId="0">
-      <selection activeCell="G1544" sqref="G1544"/>
+    <sheetView tabSelected="1" topLeftCell="A1529" workbookViewId="0">
+      <selection activeCell="C1541" sqref="C1541:D1567"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26020,7 +26020,7 @@
         <v>0</v>
       </c>
       <c r="D1541" s="5">
-        <v>140</v>
+        <v>192</v>
       </c>
     </row>
     <row r="1542" spans="2:4" x14ac:dyDescent="0.25">
@@ -26031,7 +26031,7 @@
         <v>1</v>
       </c>
       <c r="D1542" s="5">
-        <v>418</v>
+        <v>588</v>
       </c>
     </row>
     <row r="1543" spans="2:4" x14ac:dyDescent="0.25">
@@ -26042,7 +26042,7 @@
         <v>2</v>
       </c>
       <c r="D1543" s="5">
-        <v>89</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1544" spans="2:4" x14ac:dyDescent="0.25">
@@ -26053,7 +26053,7 @@
         <v>3</v>
       </c>
       <c r="D1544" s="5">
-        <v>499</v>
+        <v>654</v>
       </c>
     </row>
     <row r="1545" spans="2:4" x14ac:dyDescent="0.25">
@@ -26064,7 +26064,7 @@
         <v>4</v>
       </c>
       <c r="D1545" s="5">
-        <v>2415</v>
+        <v>3309</v>
       </c>
     </row>
     <row r="1546" spans="2:4" x14ac:dyDescent="0.25">
@@ -26075,7 +26075,7 @@
         <v>5</v>
       </c>
       <c r="D1546" s="5">
-        <v>1216</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="1547" spans="2:4" x14ac:dyDescent="0.25">
@@ -26086,7 +26086,7 @@
         <v>6</v>
       </c>
       <c r="D1547" s="5">
-        <v>560</v>
+        <v>799</v>
       </c>
     </row>
     <row r="1548" spans="2:4" x14ac:dyDescent="0.25">
@@ -26097,7 +26097,7 @@
         <v>7</v>
       </c>
       <c r="D1548" s="5">
-        <v>734</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="1549" spans="2:4" x14ac:dyDescent="0.25">
@@ -26108,7 +26108,7 @@
         <v>8</v>
       </c>
       <c r="D1549" s="5">
-        <v>1422</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="1550" spans="2:4" x14ac:dyDescent="0.25">
@@ -26119,7 +26119,7 @@
         <v>9</v>
       </c>
       <c r="D1550" s="5">
-        <v>577</v>
+        <v>908</v>
       </c>
     </row>
     <row r="1551" spans="2:4" x14ac:dyDescent="0.25">
@@ -26130,7 +26130,7 @@
         <v>10</v>
       </c>
       <c r="D1551" s="5">
-        <v>325</v>
+        <v>663</v>
       </c>
     </row>
     <row r="1552" spans="2:4" x14ac:dyDescent="0.25">
@@ -26141,7 +26141,7 @@
         <v>11</v>
       </c>
       <c r="D1552" s="5">
-        <v>585</v>
+        <v>876</v>
       </c>
     </row>
     <row r="1553" spans="2:4" x14ac:dyDescent="0.25">
@@ -26152,7 +26152,7 @@
         <v>12</v>
       </c>
       <c r="D1553" s="5">
-        <v>4054</v>
+        <v>6887</v>
       </c>
     </row>
     <row r="1554" spans="2:4" x14ac:dyDescent="0.25">
@@ -26163,7 +26163,7 @@
         <v>13</v>
       </c>
       <c r="D1554" s="5">
-        <v>2241</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="1555" spans="2:4" x14ac:dyDescent="0.25">
@@ -26174,7 +26174,7 @@
         <v>14</v>
       </c>
       <c r="D1555" s="5">
-        <v>729</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="1556" spans="2:4" x14ac:dyDescent="0.25">
@@ -26185,7 +26185,7 @@
         <v>15</v>
       </c>
       <c r="D1556" s="5">
-        <v>567</v>
+        <v>803</v>
       </c>
     </row>
     <row r="1557" spans="2:4" x14ac:dyDescent="0.25">
@@ -26196,7 +26196,7 @@
         <v>16</v>
       </c>
       <c r="D1557" s="5">
-        <v>1803</v>
+        <v>2513</v>
       </c>
     </row>
     <row r="1558" spans="2:4" x14ac:dyDescent="0.25">
@@ -26207,7 +26207,7 @@
         <v>17</v>
       </c>
       <c r="D1558" s="5">
-        <v>292</v>
+        <v>405</v>
       </c>
     </row>
     <row r="1559" spans="2:4" x14ac:dyDescent="0.25">
@@ -26218,7 +26218,7 @@
         <v>18</v>
       </c>
       <c r="D1559" s="5">
-        <v>480</v>
+        <v>643</v>
       </c>
     </row>
     <row r="1560" spans="2:4" x14ac:dyDescent="0.25">
@@ -26229,7 +26229,7 @@
         <v>19</v>
       </c>
       <c r="D1560" s="5">
-        <v>3137</v>
+        <v>4214</v>
       </c>
     </row>
     <row r="1561" spans="2:4" x14ac:dyDescent="0.25">
@@ -26240,7 +26240,7 @@
         <v>20</v>
       </c>
       <c r="D1561" s="5">
-        <v>4105</v>
+        <v>5840</v>
       </c>
     </row>
     <row r="1562" spans="2:4" x14ac:dyDescent="0.25">
@@ -26251,7 +26251,7 @@
         <v>21</v>
       </c>
       <c r="D1562" s="5">
-        <v>283</v>
+        <v>428</v>
       </c>
     </row>
     <row r="1563" spans="2:4" x14ac:dyDescent="0.25">
@@ -26262,7 +26262,7 @@
         <v>22</v>
       </c>
       <c r="D1563" s="5">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="1564" spans="2:4" x14ac:dyDescent="0.25">
@@ -26273,7 +26273,7 @@
         <v>23</v>
       </c>
       <c r="D1564" s="5">
-        <v>1410</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="1565" spans="2:4" x14ac:dyDescent="0.25">
@@ -26284,7 +26284,7 @@
         <v>24</v>
       </c>
       <c r="D1565" s="5">
-        <v>379</v>
+        <v>582</v>
       </c>
     </row>
     <row r="1566" spans="2:4" x14ac:dyDescent="0.25">
@@ -26295,7 +26295,7 @@
         <v>25</v>
       </c>
       <c r="D1566" s="5">
-        <v>10852</v>
+        <v>16207</v>
       </c>
     </row>
     <row r="1567" spans="2:4" x14ac:dyDescent="0.25">
@@ -26306,7 +26306,7 @@
         <v>26</v>
       </c>
       <c r="D1567" s="5">
-        <v>230</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>